<commit_message>
Primeiro commit da Branch
</commit_message>
<xml_diff>
--- a/Seminário 1 - CMSE/Atas - 2020 a 2023 - Dados.xlsx
+++ b/Seminário 1 - CMSE/Atas - 2020 a 2023 - Dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06eb512eaad66502/Área de Trabalho/SEMINÁRIO ATAS CMSE/Seminário 1 - CMSE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f464b536d712b41b/Engenharia Elétrica/Mestrado/01 - Disciplinas/2023.1/Planejamento Energético/Seminário 1 - CMSE/Gestao_energetica_trabalhos/Seminário 1 - CMSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4D361C20488DEA4E38A0D59CDB48AC5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A8C85A2-E605-4319-B291-99CA88AC21AB}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="11_AD4D361C20488DEA4E38A0D59CDB48AC5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71C2594D-A662-4682-961C-77C7871C3E83}"/>
   <bookViews>
-    <workbookView xWindow="-1140" yWindow="3900" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Ata</t>
   </si>
@@ -33,22 +33,19 @@
     <t>Ano</t>
   </si>
   <si>
-    <t>Nível dos reservatórios</t>
-  </si>
-  <si>
-    <t>Alertas</t>
-  </si>
-  <si>
-    <t>Dado A</t>
-  </si>
-  <si>
-    <t>Dado B</t>
-  </si>
-  <si>
     <t>Dado C</t>
   </si>
   <si>
     <t>Dado D</t>
+  </si>
+  <si>
+    <t>Km de linha</t>
+  </si>
+  <si>
+    <t>Capacidade de Transformação (MVA)</t>
+  </si>
+  <si>
+    <t>Instalação de Geração (MW)</t>
   </si>
 </sst>
 </file>
@@ -310,11 +307,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$D$1</c:f>
+              <c:f>Plan1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nível dos reservatórios</c:v>
+                  <c:v>Instalação de Geração (MW)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -495,156 +492,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$2:$D$50</c:f>
+              <c:f>Plan1!$C$2:$C$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>24</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1032,11 +888,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$E$1</c:f>
+              <c:f>Plan1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dado A</c:v>
+                  <c:v>Km de linha</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1067,156 +923,15 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$2:$E$50</c:f>
+              <c:f>Plan1!$D$2:$D$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
+                  <c:v>964</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1233,11 +948,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$F$1</c:f>
+              <c:f>Plan1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dado B</c:v>
+                  <c:v>Capacidade de Transformação (MVA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1268,156 +983,15 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$F$2:$F$50</c:f>
+              <c:f>Plan1!$E$2:$E$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1</c:v>
+                  <c:v>1466</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2714,13 +2288,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>171449</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>19049</xdr:rowOff>
@@ -2750,13 +2324,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -3050,23 +2624,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -3074,889 +2648,472 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2020</v>
       </c>
       <c r="B2" s="3">
         <v>226</v>
       </c>
+      <c r="C2" s="3">
+        <v>416</v>
+      </c>
       <c r="D2" s="3">
-        <v>20</v>
+        <v>205</v>
       </c>
       <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>49</v>
-      </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2020</v>
       </c>
       <c r="B3" s="3">
         <v>227</v>
       </c>
+      <c r="C3" s="3">
+        <v>93</v>
+      </c>
       <c r="D3" s="3">
-        <v>21</v>
+        <v>964</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>48</v>
-      </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1466</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2020</v>
       </c>
       <c r="B4" s="3">
         <v>228</v>
       </c>
-      <c r="D4" s="3">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3">
-        <v>47</v>
-      </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
       <c r="B5" s="3">
         <v>229</v>
       </c>
-      <c r="D5" s="3">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3">
-        <v>46</v>
-      </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2020</v>
       </c>
       <c r="B6" s="3">
         <v>230</v>
       </c>
-      <c r="D6" s="3">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3">
-        <v>5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>45</v>
-      </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2020</v>
       </c>
       <c r="B7" s="3">
         <v>231</v>
       </c>
-      <c r="D7" s="3">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3">
-        <v>6</v>
-      </c>
-      <c r="F7" s="3">
-        <v>44</v>
-      </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>2020</v>
       </c>
       <c r="B8" s="3">
         <v>232</v>
       </c>
-      <c r="D8" s="3">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3">
-        <v>43</v>
-      </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2020</v>
       </c>
       <c r="B9" s="3">
         <v>233</v>
       </c>
-      <c r="D9" s="3">
-        <v>22</v>
-      </c>
-      <c r="E9" s="3">
-        <v>8</v>
-      </c>
-      <c r="F9" s="3">
-        <v>42</v>
-      </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2020</v>
       </c>
       <c r="B10" s="3">
         <v>234</v>
       </c>
-      <c r="D10" s="3">
-        <v>21</v>
-      </c>
-      <c r="E10" s="3">
-        <v>9</v>
-      </c>
-      <c r="F10" s="3">
-        <v>41</v>
-      </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2020</v>
       </c>
       <c r="B11" s="3">
         <v>235</v>
       </c>
-      <c r="D11" s="3">
-        <v>20</v>
-      </c>
-      <c r="E11" s="3">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3">
-        <v>40</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2020</v>
       </c>
       <c r="B12" s="3">
         <v>236</v>
       </c>
-      <c r="D12" s="3">
-        <v>19</v>
-      </c>
-      <c r="E12" s="3">
-        <v>11</v>
-      </c>
-      <c r="F12" s="3">
-        <v>39</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>2020</v>
       </c>
       <c r="B13" s="3">
         <v>237</v>
       </c>
-      <c r="D13" s="3">
-        <v>18</v>
-      </c>
-      <c r="E13" s="3">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3">
-        <v>38</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>2020</v>
       </c>
       <c r="B14" s="3">
         <v>238</v>
       </c>
-      <c r="D14" s="3">
-        <v>17</v>
-      </c>
-      <c r="E14" s="3">
-        <v>13</v>
-      </c>
-      <c r="F14" s="3">
-        <v>37</v>
-      </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>2020</v>
       </c>
       <c r="B15" s="3">
         <v>239</v>
       </c>
-      <c r="D15" s="3">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3">
-        <v>14</v>
-      </c>
-      <c r="F15" s="3">
-        <v>36</v>
-      </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>2020</v>
       </c>
       <c r="B16" s="3">
         <v>240</v>
       </c>
-      <c r="D16" s="3">
-        <v>17</v>
-      </c>
-      <c r="E16" s="3">
-        <v>15</v>
-      </c>
-      <c r="F16" s="3">
-        <v>35</v>
-      </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>2020</v>
       </c>
       <c r="B17" s="3">
         <v>241</v>
       </c>
-      <c r="D17" s="3">
-        <v>18</v>
-      </c>
-      <c r="E17" s="3">
-        <v>16</v>
-      </c>
-      <c r="F17" s="3">
-        <v>34</v>
-      </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>2020</v>
       </c>
       <c r="B18" s="3">
         <v>242</v>
       </c>
-      <c r="D18" s="3">
-        <v>19</v>
-      </c>
-      <c r="E18" s="3">
-        <v>17</v>
-      </c>
-      <c r="F18" s="3">
-        <v>33</v>
-      </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>2021</v>
       </c>
       <c r="B19" s="3">
         <v>243</v>
       </c>
-      <c r="D19" s="3">
-        <v>20</v>
-      </c>
-      <c r="E19" s="3">
-        <v>18</v>
-      </c>
-      <c r="F19" s="3">
-        <v>32</v>
-      </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>2021</v>
       </c>
       <c r="B20" s="3">
         <v>244</v>
       </c>
-      <c r="D20" s="3">
-        <v>21</v>
-      </c>
-      <c r="E20" s="3">
-        <v>19</v>
-      </c>
-      <c r="F20" s="3">
-        <v>31</v>
-      </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>2021</v>
       </c>
       <c r="B21" s="3">
         <v>245</v>
       </c>
-      <c r="D21" s="3">
-        <v>22</v>
-      </c>
-      <c r="E21" s="3">
-        <v>20</v>
-      </c>
-      <c r="F21" s="3">
-        <v>30</v>
-      </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>2021</v>
       </c>
       <c r="B22" s="3">
         <v>246</v>
       </c>
-      <c r="D22" s="3">
-        <v>23</v>
-      </c>
-      <c r="E22" s="3">
-        <v>21</v>
-      </c>
-      <c r="F22" s="3">
-        <v>29</v>
-      </c>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>2021</v>
       </c>
       <c r="B23" s="3">
         <v>247</v>
       </c>
-      <c r="D23" s="3">
-        <v>24</v>
-      </c>
-      <c r="E23" s="3">
-        <v>22</v>
-      </c>
-      <c r="F23" s="3">
-        <v>28</v>
-      </c>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>2021</v>
       </c>
       <c r="B24" s="3">
         <v>248</v>
       </c>
-      <c r="D24" s="3">
-        <v>25</v>
-      </c>
-      <c r="E24" s="3">
-        <v>23</v>
-      </c>
-      <c r="F24" s="3">
-        <v>27</v>
-      </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>2021</v>
       </c>
       <c r="B25" s="3">
         <v>249</v>
       </c>
-      <c r="D25" s="3">
-        <v>26</v>
-      </c>
-      <c r="E25" s="3">
-        <v>24</v>
-      </c>
-      <c r="F25" s="3">
-        <v>26</v>
-      </c>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>2021</v>
       </c>
       <c r="B26" s="3">
         <v>250</v>
       </c>
-      <c r="D26" s="3">
-        <v>27</v>
-      </c>
-      <c r="E26" s="3">
-        <v>25</v>
-      </c>
-      <c r="F26" s="3">
-        <v>25</v>
-      </c>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>2021</v>
       </c>
       <c r="B27" s="3">
         <v>251</v>
       </c>
-      <c r="D27" s="3">
-        <v>28</v>
-      </c>
-      <c r="E27" s="3">
-        <v>26</v>
-      </c>
-      <c r="F27" s="3">
-        <v>24</v>
-      </c>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>2021</v>
       </c>
       <c r="B28" s="3">
         <v>252</v>
       </c>
-      <c r="D28" s="3">
-        <v>29</v>
-      </c>
-      <c r="E28" s="3">
-        <v>27</v>
-      </c>
-      <c r="F28" s="3">
-        <v>23</v>
-      </c>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>2021</v>
       </c>
       <c r="B29" s="3">
         <v>253</v>
       </c>
-      <c r="D29" s="3">
-        <v>30</v>
-      </c>
-      <c r="E29" s="3">
-        <v>28</v>
-      </c>
-      <c r="F29" s="3">
-        <v>22</v>
-      </c>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>2021</v>
       </c>
       <c r="B30" s="3">
         <v>254</v>
       </c>
-      <c r="D30" s="3">
-        <v>31</v>
-      </c>
-      <c r="E30" s="3">
-        <v>29</v>
-      </c>
-      <c r="F30" s="3">
-        <v>21</v>
-      </c>
-      <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>2021</v>
       </c>
       <c r="B31" s="3">
         <v>255</v>
       </c>
-      <c r="D31" s="3">
-        <v>32</v>
-      </c>
-      <c r="E31" s="3">
-        <v>30</v>
-      </c>
-      <c r="F31" s="3">
-        <v>20</v>
-      </c>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>2021</v>
       </c>
       <c r="B32" s="3">
         <v>256</v>
       </c>
-      <c r="D32" s="3">
-        <v>31</v>
-      </c>
-      <c r="E32" s="3">
-        <v>31</v>
-      </c>
-      <c r="F32" s="3">
-        <v>19</v>
-      </c>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>2021</v>
       </c>
       <c r="B33" s="3">
         <v>257</v>
       </c>
-      <c r="D33" s="3">
-        <v>28</v>
-      </c>
-      <c r="E33" s="3">
-        <v>32</v>
-      </c>
-      <c r="F33" s="3">
-        <v>18</v>
-      </c>
-      <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>2021</v>
       </c>
       <c r="B34" s="3">
         <v>258</v>
       </c>
-      <c r="D34" s="3">
-        <v>27</v>
-      </c>
-      <c r="E34" s="3">
-        <v>33</v>
-      </c>
-      <c r="F34" s="3">
-        <v>17</v>
-      </c>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>2021</v>
       </c>
       <c r="B35" s="3">
         <v>259</v>
       </c>
-      <c r="D35" s="3">
-        <v>26</v>
-      </c>
-      <c r="E35" s="3">
-        <v>34</v>
-      </c>
-      <c r="F35" s="3">
-        <v>16</v>
-      </c>
-      <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>2022</v>
       </c>
       <c r="B36" s="3">
         <v>260</v>
       </c>
-      <c r="D36" s="3">
-        <v>25</v>
-      </c>
-      <c r="E36" s="3">
-        <v>35</v>
-      </c>
-      <c r="F36" s="3">
-        <v>15</v>
-      </c>
-      <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>2022</v>
       </c>
       <c r="B37" s="3">
         <v>261</v>
       </c>
-      <c r="D37" s="3">
-        <v>24</v>
-      </c>
-      <c r="E37" s="3">
-        <v>36</v>
-      </c>
-      <c r="F37" s="3">
-        <v>14</v>
-      </c>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>2022</v>
       </c>
       <c r="B38" s="3">
         <v>262</v>
       </c>
-      <c r="D38" s="3">
-        <v>23</v>
-      </c>
-      <c r="E38" s="3">
-        <v>37</v>
-      </c>
-      <c r="F38" s="3">
-        <v>13</v>
-      </c>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>2022</v>
       </c>
       <c r="B39" s="3">
         <v>263</v>
       </c>
-      <c r="D39" s="3">
-        <v>22</v>
-      </c>
-      <c r="E39" s="3">
-        <v>38</v>
-      </c>
-      <c r="F39" s="3">
-        <v>12</v>
-      </c>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>2022</v>
       </c>
       <c r="B40" s="3">
         <v>264</v>
       </c>
-      <c r="D40" s="3">
-        <v>21</v>
-      </c>
-      <c r="E40" s="3">
-        <v>39</v>
-      </c>
-      <c r="F40" s="3">
-        <v>11</v>
-      </c>
-      <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>2022</v>
       </c>
       <c r="B41" s="3">
         <v>265</v>
       </c>
-      <c r="D41" s="3">
-        <v>20</v>
-      </c>
-      <c r="E41" s="3">
-        <v>40</v>
-      </c>
-      <c r="F41" s="3">
-        <v>10</v>
-      </c>
-      <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>2022</v>
       </c>
       <c r="B42" s="3">
         <v>266</v>
       </c>
-      <c r="D42" s="3">
-        <v>19</v>
-      </c>
-      <c r="E42" s="3">
-        <v>41</v>
-      </c>
-      <c r="F42" s="3">
-        <v>9</v>
-      </c>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>2022</v>
       </c>
       <c r="B43" s="3">
         <v>267</v>
       </c>
-      <c r="D43" s="3">
-        <v>20</v>
-      </c>
-      <c r="E43" s="3">
-        <v>42</v>
-      </c>
-      <c r="F43" s="3">
-        <v>8</v>
-      </c>
-      <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>2022</v>
       </c>
       <c r="B44" s="3">
         <v>268</v>
       </c>
-      <c r="D44" s="3">
-        <v>21</v>
-      </c>
-      <c r="E44" s="3">
-        <v>43</v>
-      </c>
-      <c r="F44" s="3">
-        <v>7</v>
-      </c>
-      <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>2022</v>
       </c>
       <c r="B45" s="3">
         <v>269</v>
       </c>
-      <c r="D45" s="3">
-        <v>21</v>
-      </c>
-      <c r="E45" s="3">
-        <v>44</v>
-      </c>
-      <c r="F45" s="3">
-        <v>6</v>
-      </c>
-      <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>2022</v>
       </c>
       <c r="B46" s="3">
         <v>270</v>
       </c>
-      <c r="D46" s="3">
-        <v>22</v>
-      </c>
-      <c r="E46" s="3">
-        <v>45</v>
-      </c>
-      <c r="F46" s="3">
-        <v>5</v>
-      </c>
-      <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>2022</v>
       </c>
       <c r="B47" s="3">
         <v>271</v>
       </c>
-      <c r="D47" s="3">
-        <v>23</v>
-      </c>
-      <c r="E47" s="3">
-        <v>46</v>
-      </c>
-      <c r="F47" s="3">
-        <v>4</v>
-      </c>
-      <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>2022</v>
       </c>
       <c r="B48" s="3">
         <v>272</v>
       </c>
-      <c r="D48" s="3">
-        <v>24</v>
-      </c>
-      <c r="E48" s="3">
-        <v>47</v>
-      </c>
-      <c r="F48" s="3">
-        <v>3</v>
-      </c>
-      <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>2023</v>
       </c>
       <c r="B49" s="3">
         <v>273</v>
       </c>
-      <c r="D49" s="3">
-        <v>24</v>
-      </c>
-      <c r="E49" s="3">
-        <v>48</v>
-      </c>
-      <c r="F49" s="3">
-        <v>2</v>
-      </c>
-      <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>2023</v>
       </c>
@@ -3964,17 +3121,10 @@
         <v>274</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="7">
-        <v>24</v>
-      </c>
-      <c r="E50" s="7">
-        <v>49</v>
-      </c>
-      <c r="F50" s="7">
-        <v>1</v>
-      </c>
-      <c r="G50" s="7"/>
-      <c r="H50" s="8"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adicionando rascunho da apresentação
</commit_message>
<xml_diff>
--- a/Seminário 1 - CMSE/Atas - 2020 a 2023 - Dados.xlsx
+++ b/Seminário 1 - CMSE/Atas - 2020 a 2023 - Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f464b536d712b41b/Engenharia Elétrica/Mestrado/01 - Disciplinas/2023.1/Planejamento Energético/Seminário 1 - CMSE/Gestao_energetica_trabalhos/Seminário 1 - CMSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="11_AD4D361C20488DEA4E38A0D59CDB48AC5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71C2594D-A662-4682-961C-77C7871C3E83}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="11_AD4D361C20488DEA4E38A0D59CDB48AC5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCA5CA7B-258A-458B-96E8-660447B0FA6D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
   <si>
     <t>Ata</t>
   </si>
   <si>
     <t>Ano</t>
-  </si>
-  <si>
-    <t>Dado C</t>
   </si>
   <si>
     <t>Dado D</t>
@@ -46,6 +43,51 @@
   </si>
   <si>
     <t>Instalação de Geração (MW)</t>
+  </si>
+  <si>
+    <t>GD (MW)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>236*</t>
+  </si>
+  <si>
+    <t>* Extraordinária</t>
+  </si>
+  <si>
+    <t>237*</t>
+  </si>
+  <si>
+    <t>238*</t>
+  </si>
+  <si>
+    <t>239*</t>
+  </si>
+  <si>
+    <t>240*</t>
+  </si>
+  <si>
+    <t>241*</t>
+  </si>
+  <si>
+    <t>248*</t>
+  </si>
+  <si>
+    <t>252*</t>
+  </si>
+  <si>
+    <t>253*</t>
+  </si>
+  <si>
+    <t>UTE GNA I,</t>
+  </si>
+  <si>
+    <t>256*</t>
+  </si>
+  <si>
+    <t>259*</t>
   </si>
 </sst>
 </file>
@@ -194,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -228,6 +270,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -335,10 +380,9 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Plan1!$B$2:$B$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>226</c:v>
@@ -371,22 +415,22 @@
                   <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>236</c:v>
+                  <c:v>236*</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>237</c:v>
+                  <c:v>237*</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>238</c:v>
+                  <c:v>238*</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>239</c:v>
+                  <c:v>239*</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>240</c:v>
+                  <c:v>240*</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>241</c:v>
+                  <c:v>241*</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>242</c:v>
@@ -407,7 +451,7 @@
                   <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>248</c:v>
+                  <c:v>248*</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>249</c:v>
@@ -419,10 +463,10 @@
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>252</c:v>
+                  <c:v>252*</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>253</c:v>
+                  <c:v>253*</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>254</c:v>
@@ -431,7 +475,7 @@
                   <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>256</c:v>
+                  <c:v>256*</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>257</c:v>
@@ -440,7 +484,7 @@
                   <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>259</c:v>
+                  <c:v>259*</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>260</c:v>
@@ -487,8 +531,8 @@
                 <c:pt idx="48">
                   <c:v>274</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -501,6 +545,99 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1606</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>791</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1770</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>984</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -933,6 +1070,99 @@
                 <c:pt idx="1">
                   <c:v>964</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>878</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1193</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>74.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1132.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>446</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>295</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -992,6 +1222,99 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1466</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1344</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1167</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3962</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4350</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1041</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2361,6 +2684,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2624,10 +2951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,7 +2964,9 @@
     <col min="3" max="3" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="14.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2648,19 +2977,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2706,6 +3035,15 @@
       <c r="B4" s="3">
         <v>228</v>
       </c>
+      <c r="C4" s="3">
+        <v>197</v>
+      </c>
+      <c r="D4" s="3">
+        <v>211</v>
+      </c>
+      <c r="E4" s="3">
+        <v>750</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2715,6 +3053,18 @@
       <c r="B5" s="3">
         <v>229</v>
       </c>
+      <c r="C5" s="3">
+        <v>1606</v>
+      </c>
+      <c r="D5" s="3">
+        <v>878</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1344</v>
+      </c>
+      <c r="F5" s="3">
+        <v>182</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2724,6 +3074,18 @@
       <c r="B6" s="3">
         <v>230</v>
       </c>
+      <c r="C6" s="3">
+        <v>345</v>
+      </c>
+      <c r="D6" s="3">
+        <v>166</v>
+      </c>
+      <c r="E6" s="3">
+        <v>125</v>
+      </c>
+      <c r="F6" s="3">
+        <v>250</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2733,6 +3095,18 @@
       <c r="B7" s="3">
         <v>231</v>
       </c>
+      <c r="C7" s="3">
+        <v>494</v>
+      </c>
+      <c r="D7" s="3">
+        <v>686</v>
+      </c>
+      <c r="E7" s="3">
+        <v>166</v>
+      </c>
+      <c r="F7" s="3">
+        <v>91</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2742,6 +3116,18 @@
       <c r="B8" s="3">
         <v>232</v>
       </c>
+      <c r="C8" s="3">
+        <v>133</v>
+      </c>
+      <c r="D8" s="3">
+        <v>146</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1167</v>
+      </c>
+      <c r="F8" s="3">
+        <v>144</v>
+      </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2751,6 +3137,18 @@
       <c r="B9" s="3">
         <v>233</v>
       </c>
+      <c r="C9" s="3">
+        <v>120</v>
+      </c>
+      <c r="D9" s="3">
+        <v>336</v>
+      </c>
+      <c r="E9" s="3">
+        <v>99</v>
+      </c>
+      <c r="F9" s="3">
+        <v>229</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2760,6 +3158,18 @@
       <c r="B10" s="3">
         <v>234</v>
       </c>
+      <c r="C10" s="3">
+        <v>173</v>
+      </c>
+      <c r="D10" s="3">
+        <v>172</v>
+      </c>
+      <c r="E10" s="3">
+        <v>850</v>
+      </c>
+      <c r="F10" s="3">
+        <v>237</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2769,14 +3179,38 @@
       <c r="B11" s="3">
         <v>235</v>
       </c>
+      <c r="C11" s="3">
+        <v>160</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>375</v>
+      </c>
+      <c r="F11" s="3">
+        <v>283</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>2020</v>
       </c>
-      <c r="B12" s="3">
-        <v>236</v>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -2784,8 +3218,20 @@
       <c r="A13" s="4">
         <v>2020</v>
       </c>
-      <c r="B13" s="3">
-        <v>237</v>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>323</v>
+      </c>
+      <c r="D13" s="3">
+        <v>350</v>
+      </c>
+      <c r="E13" s="3">
+        <v>300</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G13" s="5"/>
     </row>
@@ -2793,8 +3239,20 @@
       <c r="A14" s="4">
         <v>2020</v>
       </c>
-      <c r="B14" s="3">
-        <v>238</v>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -2802,8 +3260,20 @@
       <c r="A15" s="4">
         <v>2020</v>
       </c>
-      <c r="B15" s="3">
-        <v>239</v>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -2811,8 +3281,20 @@
       <c r="A16" s="4">
         <v>2020</v>
       </c>
-      <c r="B16" s="3">
-        <v>240</v>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G16" s="5"/>
     </row>
@@ -2820,19 +3302,43 @@
       <c r="A17" s="4">
         <v>2020</v>
       </c>
-      <c r="B17" s="3">
-        <v>241</v>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="6">
         <v>2020</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="7">
         <v>242</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="C18" s="7">
+        <v>302</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1193</v>
+      </c>
+      <c r="E18" s="7">
+        <v>3962</v>
+      </c>
+      <c r="F18" s="7">
+        <v>204</v>
+      </c>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -2841,6 +3347,18 @@
       <c r="B19" s="3">
         <v>243</v>
       </c>
+      <c r="C19" s="3">
+        <v>791</v>
+      </c>
+      <c r="D19" s="3">
+        <v>352</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2850,6 +3368,18 @@
       <c r="B20" s="3">
         <v>244</v>
       </c>
+      <c r="C20" s="3">
+        <v>144</v>
+      </c>
+      <c r="D20" s="3">
+        <v>499</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1208</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2859,6 +3389,18 @@
       <c r="B21" s="3">
         <v>245</v>
       </c>
+      <c r="C21" s="3">
+        <v>130</v>
+      </c>
+      <c r="D21" s="3">
+        <v>74.3</v>
+      </c>
+      <c r="E21" s="3">
+        <v>800</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2868,6 +3410,18 @@
       <c r="B22" s="3">
         <v>246</v>
       </c>
+      <c r="C22" s="3">
+        <v>388</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1132.8</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4350</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2877,14 +3431,38 @@
       <c r="B23" s="3">
         <v>247</v>
       </c>
+      <c r="C23" s="3">
+        <v>620</v>
+      </c>
+      <c r="D23" s="3">
+        <v>400</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1600</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>2021</v>
       </c>
-      <c r="B24" s="3">
-        <v>248</v>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G24" s="5"/>
     </row>
@@ -2895,6 +3473,18 @@
       <c r="B25" s="3">
         <v>249</v>
       </c>
+      <c r="C25" s="3">
+        <v>244</v>
+      </c>
+      <c r="D25" s="3">
+        <v>79</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1041</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2904,6 +3494,18 @@
       <c r="B26" s="3">
         <v>250</v>
       </c>
+      <c r="C26" s="3">
+        <v>426</v>
+      </c>
+      <c r="D26" s="3">
+        <v>179</v>
+      </c>
+      <c r="E26" s="3">
+        <v>772</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2913,14 +3515,38 @@
       <c r="B27" s="3">
         <v>251</v>
       </c>
+      <c r="C27" s="3">
+        <v>477</v>
+      </c>
+      <c r="D27" s="3">
+        <v>446</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>2021</v>
       </c>
-      <c r="B28" s="3">
-        <v>252</v>
+      <c r="B28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G28" s="5"/>
     </row>
@@ -2928,8 +3554,20 @@
       <c r="A29" s="4">
         <v>2021</v>
       </c>
-      <c r="B29" s="3">
-        <v>253</v>
+      <c r="B29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G29" s="5"/>
     </row>
@@ -2940,6 +3578,18 @@
       <c r="B30" s="3">
         <v>254</v>
       </c>
+      <c r="C30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2949,14 +3599,40 @@
       <c r="B31" s="3">
         <v>255</v>
       </c>
-      <c r="G31" s="5"/>
+      <c r="C31" s="3">
+        <v>1770</v>
+      </c>
+      <c r="D31" s="3">
+        <v>596</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>2021</v>
       </c>
-      <c r="B32" s="3">
-        <v>256</v>
+      <c r="B32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G32" s="5"/>
     </row>
@@ -2967,6 +3643,18 @@
       <c r="B33" s="3">
         <v>257</v>
       </c>
+      <c r="C33" s="3">
+        <v>984</v>
+      </c>
+      <c r="D33" s="3">
+        <v>156</v>
+      </c>
+      <c r="E33" s="3">
+        <v>300</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2976,16 +3664,32 @@
       <c r="B34" s="3">
         <v>258</v>
       </c>
+      <c r="C34" s="3">
+        <v>496</v>
+      </c>
+      <c r="D34" s="3">
+        <v>295</v>
+      </c>
+      <c r="E34" s="3">
+        <v>700</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="6">
         <v>2021</v>
       </c>
-      <c r="B35" s="3">
-        <v>259</v>
-      </c>
-      <c r="G35" s="5"/>
+      <c r="B35" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
@@ -3096,13 +3800,17 @@
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="A48" s="6">
         <v>2022</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="7">
         <v>272</v>
       </c>
-      <c r="G48" s="5"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
@@ -3126,6 +3834,11 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizando rastreamento de ações tomadas pelo CMSE até a reunião 275
</commit_message>
<xml_diff>
--- a/Seminário 1 - CMSE/Atas - 2020 a 2023 - Dados.xlsx
+++ b/Seminário 1 - CMSE/Atas - 2020 a 2023 - Dados.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f464b536d712b41b/Engenharia Elétrica/Mestrado/01 - Disciplinas/2023.1/Planejamento Energético/Seminário 1 - CMSE/Gestao_energetica_trabalhos/Seminário 1 - CMSE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="11_AD4D361C20488DEA4E38A0D59CDB48AC5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CCA5CA7B-258A-458B-96E8-660447B0FA6D}"/>
+  <xr:revisionPtr revIDLastSave="306" documentId="11_AD4D361C20488DEA4E38A0D59CDB48AC5BDEDD8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C8D5E64-DD75-44C9-B186-E3C18857E5C9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="22">
   <si>
     <t>Ata</t>
   </si>
@@ -88,6 +99,9 @@
   </si>
   <si>
     <t>259*</t>
+  </si>
+  <si>
+    <t>262*</t>
   </si>
 </sst>
 </file>
@@ -236,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -273,6 +287,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -381,9 +401,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Plan1!$B$2:$B$50</c:f>
+              <c:f>Plan1!$B$2:$B$51</c:f>
               <c:strCache>
-                <c:ptCount val="49"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>226</c:v>
                 </c:pt>
@@ -493,7 +513,7 @@
                   <c:v>261</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>262</c:v>
+                  <c:v>262*</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>263</c:v>
@@ -530,16 +550,19 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>275</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$C$2:$C$50</c:f>
+              <c:f>Plan1!$C$2:$C$51</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>416</c:v>
                 </c:pt>
@@ -638,6 +661,57 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>516</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1387</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>941</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1030</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2138</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -843,7 +917,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1060,10 +1134,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$2:$D$50</c:f>
+              <c:f>Plan1!$D$2:$D$51</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>205</c:v>
                 </c:pt>
@@ -1162,6 +1236,57 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1213</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>409</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1012</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>544</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1223</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1213,10 +1338,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$E$2:$E$50</c:f>
+              <c:f>Plan1!$E$2:$E$51</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>322</c:v>
                 </c:pt>
@@ -1315,6 +1440,57 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2396</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2226</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1866</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1410,7 +1586,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2951,10 +3127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2999,15 +3175,16 @@
       <c r="B2" s="3">
         <v>226</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="13">
         <v>416</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="13">
         <v>205</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="13">
         <v>322</v>
       </c>
+      <c r="F2" s="13"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3017,15 +3194,16 @@
       <c r="B3" s="3">
         <v>227</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="13">
         <v>93</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="13">
         <v>964</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="13">
         <v>1466</v>
       </c>
+      <c r="F3" s="13"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3035,15 +3213,16 @@
       <c r="B4" s="3">
         <v>228</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="13">
         <v>197</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="13">
         <v>211</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="13">
         <v>750</v>
       </c>
+      <c r="F4" s="13"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3053,16 +3232,16 @@
       <c r="B5" s="3">
         <v>229</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="13">
         <v>1606</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="13">
         <v>878</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="13">
         <v>1344</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="13">
         <v>182</v>
       </c>
       <c r="G5" s="5"/>
@@ -3074,16 +3253,16 @@
       <c r="B6" s="3">
         <v>230</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="13">
         <v>345</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="13">
         <v>166</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="13">
         <v>125</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="13">
         <v>250</v>
       </c>
       <c r="G6" s="5"/>
@@ -3095,16 +3274,16 @@
       <c r="B7" s="3">
         <v>231</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="13">
         <v>494</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="13">
         <v>686</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="13">
         <v>166</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="13">
         <v>91</v>
       </c>
       <c r="G7" s="5"/>
@@ -3116,16 +3295,16 @@
       <c r="B8" s="3">
         <v>232</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="13">
         <v>133</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="13">
         <v>146</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="13">
         <v>1167</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="13">
         <v>144</v>
       </c>
       <c r="G8" s="5"/>
@@ -3137,16 +3316,16 @@
       <c r="B9" s="3">
         <v>233</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="13">
         <v>120</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="13">
         <v>336</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="13">
         <v>99</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="13">
         <v>229</v>
       </c>
       <c r="G9" s="5"/>
@@ -3158,16 +3337,16 @@
       <c r="B10" s="3">
         <v>234</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="13">
         <v>173</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="13">
         <v>172</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="13">
         <v>850</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="13">
         <v>237</v>
       </c>
       <c r="G10" s="5"/>
@@ -3179,16 +3358,16 @@
       <c r="B11" s="3">
         <v>235</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="13">
         <v>160</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="D11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="13">
         <v>375</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="13">
         <v>283</v>
       </c>
       <c r="G11" s="5"/>
@@ -3200,16 +3379,16 @@
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="C12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="5"/>
@@ -3221,16 +3400,16 @@
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="13">
         <v>323</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="13">
         <v>350</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="13">
         <v>300</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="5"/>
@@ -3242,16 +3421,16 @@
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="C14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="5"/>
@@ -3263,16 +3442,16 @@
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="C15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="5"/>
@@ -3284,16 +3463,16 @@
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="C16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="5"/>
@@ -3305,16 +3484,16 @@
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="C17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="5"/>
@@ -3326,16 +3505,16 @@
       <c r="B18" s="7">
         <v>242</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="14">
         <v>302</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="14">
         <v>1193</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="14">
         <v>3962</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="14">
         <v>204</v>
       </c>
       <c r="G18" s="8"/>
@@ -3347,16 +3526,16 @@
       <c r="B19" s="3">
         <v>243</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="13">
         <v>791</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="13">
         <v>352</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="13">
         <v>1500</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="5"/>
@@ -3368,16 +3547,16 @@
       <c r="B20" s="3">
         <v>244</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="13">
         <v>144</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="13">
         <v>499</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="13">
         <v>1208</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G20" s="5"/>
@@ -3389,16 +3568,16 @@
       <c r="B21" s="3">
         <v>245</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="13">
         <v>130</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="13">
         <v>74.3</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="13">
         <v>800</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G21" s="5"/>
@@ -3410,16 +3589,16 @@
       <c r="B22" s="3">
         <v>246</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="13">
         <v>388</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="13">
         <v>1132.8</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="13">
         <v>4350</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G22" s="5"/>
@@ -3431,16 +3610,16 @@
       <c r="B23" s="3">
         <v>247</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="13">
         <v>620</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="13">
         <v>400</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="13">
         <v>1600</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G23" s="5"/>
@@ -3452,16 +3631,16 @@
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="C24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="5"/>
@@ -3473,16 +3652,16 @@
       <c r="B25" s="3">
         <v>249</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="13">
         <v>244</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="13">
         <v>79</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="13">
         <v>1041</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G25" s="5"/>
@@ -3494,16 +3673,16 @@
       <c r="B26" s="3">
         <v>250</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="13">
         <v>426</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="13">
         <v>179</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="13">
         <v>772</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G26" s="5"/>
@@ -3515,16 +3694,16 @@
       <c r="B27" s="3">
         <v>251</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="13">
         <v>477</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="13">
         <v>446</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="E27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G27" s="5"/>
@@ -3536,16 +3715,16 @@
       <c r="B28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="C28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G28" s="5"/>
@@ -3557,16 +3736,16 @@
       <c r="B29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="3" t="s">
+      <c r="C29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G29" s="5"/>
@@ -3578,16 +3757,16 @@
       <c r="B30" s="3">
         <v>254</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="C30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="5"/>
@@ -3599,16 +3778,16 @@
       <c r="B31" s="3">
         <v>255</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="13">
         <v>1770</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="13">
         <v>596</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="13">
         <v>1200</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G31" s="5" t="s">
@@ -3622,16 +3801,16 @@
       <c r="B32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="C32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G32" s="5"/>
@@ -3643,16 +3822,16 @@
       <c r="B33" s="3">
         <v>257</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="13">
         <v>984</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="13">
         <v>156</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="13">
         <v>300</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G33" s="5"/>
@@ -3664,16 +3843,16 @@
       <c r="B34" s="3">
         <v>258</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="13">
         <v>496</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="13">
         <v>295</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="13">
         <v>700</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="13" t="s">
         <v>7</v>
       </c>
       <c r="G34" s="5"/>
@@ -3685,10 +3864,18 @@
       <c r="B35" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="C35" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3698,6 +3885,18 @@
       <c r="B36" s="3">
         <v>260</v>
       </c>
+      <c r="C36" s="13">
+        <v>1122</v>
+      </c>
+      <c r="D36" s="13">
+        <v>1213</v>
+      </c>
+      <c r="E36" s="13">
+        <v>450</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3707,14 +3906,38 @@
       <c r="B37" s="3">
         <v>261</v>
       </c>
+      <c r="C37" s="13">
+        <v>482</v>
+      </c>
+      <c r="D37" s="13">
+        <v>687</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>2022</v>
       </c>
-      <c r="B38" s="3">
-        <v>262</v>
+      <c r="B38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="G38" s="5"/>
     </row>
@@ -3725,6 +3948,18 @@
       <c r="B39" s="3">
         <v>263</v>
       </c>
+      <c r="C39" s="13">
+        <v>516</v>
+      </c>
+      <c r="D39" s="13">
+        <v>566</v>
+      </c>
+      <c r="E39" s="13">
+        <v>2396</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3734,6 +3969,18 @@
       <c r="B40" s="3">
         <v>264</v>
       </c>
+      <c r="C40" s="13">
+        <v>347</v>
+      </c>
+      <c r="D40" s="13">
+        <v>409</v>
+      </c>
+      <c r="E40" s="13">
+        <v>2226</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3743,6 +3990,18 @@
       <c r="B41" s="3">
         <v>265</v>
       </c>
+      <c r="C41" s="13">
+        <v>223</v>
+      </c>
+      <c r="D41" s="13">
+        <v>645</v>
+      </c>
+      <c r="E41" s="13">
+        <v>400</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3752,6 +4011,18 @@
       <c r="B42" s="3">
         <v>266</v>
       </c>
+      <c r="C42" s="13">
+        <v>596</v>
+      </c>
+      <c r="D42" s="13">
+        <v>1012</v>
+      </c>
+      <c r="E42" s="13">
+        <v>1250</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3761,6 +4032,18 @@
       <c r="B43" s="3">
         <v>267</v>
       </c>
+      <c r="C43" s="13">
+        <v>158</v>
+      </c>
+      <c r="D43" s="13">
+        <v>303</v>
+      </c>
+      <c r="E43" s="13">
+        <v>700</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3770,6 +4053,18 @@
       <c r="B44" s="3">
         <v>268</v>
       </c>
+      <c r="C44" s="13">
+        <v>510</v>
+      </c>
+      <c r="D44" s="13">
+        <v>544</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3779,6 +4074,18 @@
       <c r="B45" s="3">
         <v>269</v>
       </c>
+      <c r="C45" s="13">
+        <v>650</v>
+      </c>
+      <c r="D45" s="13">
+        <v>139</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3788,6 +4095,18 @@
       <c r="B46" s="3">
         <v>270</v>
       </c>
+      <c r="C46" s="13">
+        <v>1387</v>
+      </c>
+      <c r="D46" s="13">
+        <v>244</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3797,6 +4116,18 @@
       <c r="B47" s="3">
         <v>271</v>
       </c>
+      <c r="C47" s="13">
+        <v>941</v>
+      </c>
+      <c r="D47" s="13">
+        <v>152</v>
+      </c>
+      <c r="E47" s="13">
+        <v>300</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3806,10 +4137,18 @@
       <c r="B48" s="7">
         <v>272</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="C48" s="14">
+        <v>1030</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1223</v>
+      </c>
+      <c r="E48" s="14">
+        <v>750</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3819,28 +4158,68 @@
       <c r="B49" s="3">
         <v>273</v>
       </c>
+      <c r="C49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6">
+      <c r="A50" s="4">
         <v>2023</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="3">
         <v>274</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="12" t="s">
+      <c r="C50" s="13">
+        <v>2138</v>
+      </c>
+      <c r="D50" s="13">
+        <v>455</v>
+      </c>
+      <c r="E50" s="13">
+        <v>1866</v>
+      </c>
+      <c r="F50" s="13">
+        <v>864</v>
+      </c>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B51" s="7">
+        <v>275</v>
+      </c>
+      <c r="C51" s="14">
+        <v>749</v>
+      </c>
+      <c r="D51" s="14">
+        <v>1096</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>